<commit_message>
Sub categories and categories added
</commit_message>
<xml_diff>
--- a/static/exel_files/category.xlsx
+++ b/static/exel_files/category.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22821"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\DjangoRepos\Elkomerc\static\exel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CA26E8-E4EF-4F05-BD5D-67CAC3A96251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92B0EF04-0A6B-4A0A-8C22-EF98346CE68D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6450" yWindow="2595" windowWidth="14715" windowHeight="11385" xr2:uid="{B8F8F21A-1EA8-42DE-9240-0188B1CDECA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,28 +33,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>id</t>
+  </si>
   <si>
     <t>category_name</t>
   </si>
   <si>
-    <t>Kabal</t>
+    <t>Kablovi</t>
+  </si>
+  <si>
+    <t>Kablovski pribor i oprema</t>
+  </si>
+  <si>
+    <t>Kablovski nosači, kanalice</t>
   </si>
   <si>
     <t>Rasveta</t>
   </si>
   <si>
-    <t>Sklopka</t>
-  </si>
-  <si>
-    <t>id</t>
+    <t>Led rasveta</t>
+  </si>
+  <si>
+    <t>Prekidači i utičnice</t>
+  </si>
+  <si>
+    <t>Utikaci i razdelnici</t>
+  </si>
+  <si>
+    <t>Osigurači</t>
+  </si>
+  <si>
+    <t>Sklopke</t>
+  </si>
+  <si>
+    <t>Releji</t>
+  </si>
+  <si>
+    <t>Ormani i razvodne kutije</t>
+  </si>
+  <si>
+    <t>Senzori i signalizacija</t>
+  </si>
+  <si>
+    <t>Razno</t>
+  </si>
+  <si>
+    <t>Alati</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalan" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -397,48 +432,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95072704-9F27-48AB-9CF8-B7C13B46A03A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>